<commit_message>
update script A and its result
</commit_message>
<xml_diff>
--- a/2_職災分析/圖表輸出/A_整理好的資料表.xlsx
+++ b/2_職災分析/圖表輸出/A_整理好的資料表.xlsx
@@ -522,521 +522,521 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col width="9.10" max="1" min="1"/>
-    <col width="9.10" max="2" min="2"/>
-    <col width="9.10" max="3" min="3"/>
+    <col min="1" width="9.10" max="1"/>
+    <col min="2" width="9.10" max="2"/>
+    <col min="3" width="9.10" max="3"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="B1" s="1">
+    <row r="1" spans="1:3">
+      <c s="1" r="B1" t="s">
         <v>6</v>
       </c>
-      <c t="s" r="C1" s="1">
+      <c s="1" r="C1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row spans="1:3" r="2">
-      <c t="s" r="A2" s="1">
+    <row r="2" spans="1:3">
+      <c s="1" r="A2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row spans="1:3" r="3">
-      <c t="s" r="A3" s="1">
+    <row r="3" spans="1:3">
+      <c s="1" r="A3" t="s">
         <v>36</v>
       </c>
-      <c t="n" r="B3">
+      <c r="B3" t="n">
         <v>93.54838709677419</v>
       </c>
-      <c t="n" r="C3">
+      <c r="C3" t="n">
         <v>2.7909027733200857</v>
       </c>
     </row>
-    <row spans="1:3" r="4">
-      <c t="s" r="A4" s="1">
+    <row r="4" spans="1:3">
+      <c s="1" r="A4" t="s">
         <v>28</v>
       </c>
-      <c t="n" r="B4">
+      <c r="B4" t="n">
         <v>72.82608695652173</v>
       </c>
-      <c t="n" r="C4">
+      <c r="C4" t="n">
         <v>1.1850306922949305</v>
       </c>
     </row>
-    <row spans="1:3" r="5">
-      <c t="s" r="A5" s="1">
+    <row r="5" spans="1:3">
+      <c s="1" r="A5" t="s">
         <v>46</v>
       </c>
-      <c t="n" r="B5">
+      <c r="B5" t="n">
         <v>89.95901639344262</v>
       </c>
-      <c t="n" r="C5">
+      <c r="C5" t="n">
         <v>3.2985968593609494</v>
       </c>
     </row>
-    <row spans="1:3" r="6">
-      <c t="s" r="A6" s="1">
+    <row r="6" spans="1:3">
+      <c s="1" r="A6" t="s">
         <v>47</v>
       </c>
-      <c t="n" r="B6">
+      <c r="B6" t="n">
         <v>94.98207885304659</v>
       </c>
-      <c t="n" r="C6">
+      <c r="C6" t="n">
         <v>1.4449399560981002</v>
       </c>
     </row>
-    <row spans="1:3" r="7">
-      <c t="s" r="A7" s="1">
+    <row r="7" spans="1:3">
+      <c s="1" r="A7" t="s">
         <v>31</v>
       </c>
-      <c t="n" r="B7">
+      <c r="B7" t="n">
         <v>93.33333333333333</v>
       </c>
-      <c t="n" r="C7">
+      <c r="C7" t="n">
         <v>2.2512817672741976</v>
       </c>
     </row>
-    <row spans="1:3" r="8">
-      <c t="s" r="A8" s="1">
+    <row r="8" spans="1:3">
+      <c s="1" r="A8" t="s">
         <v>30</v>
       </c>
-      <c t="n" r="B8">
+      <c r="B8" t="n">
         <v>82.31797919762258</v>
       </c>
-      <c t="n" r="C8">
+      <c r="C8" t="n">
         <v>1.954265298281491</v>
       </c>
     </row>
-    <row spans="1:3" r="9">
-      <c t="s" r="A9" s="1">
+    <row r="9" spans="1:3">
+      <c s="1" r="A9" t="s">
         <v>15</v>
       </c>
-      <c t="n" r="B9">
+      <c r="B9" t="n">
         <v>85.13513513513513</v>
       </c>
-      <c t="n" r="C9">
+      <c r="C9" t="n">
         <v>1.0687829226247203</v>
       </c>
     </row>
-    <row spans="1:3" r="10">
-      <c t="s" r="A10" s="1">
+    <row r="10" spans="1:3">
+      <c s="1" r="A10" t="s">
         <v>26</v>
       </c>
-      <c t="n" r="B10">
+      <c r="B10" t="n">
         <v>84.90566037735849</v>
       </c>
-      <c t="n" r="C10">
+      <c r="C10" t="n">
         <v>2.479000948035583</v>
       </c>
     </row>
-    <row spans="1:3" r="11">
-      <c t="s" r="A11" s="1">
+    <row r="11" spans="1:3">
+      <c s="1" r="A11" t="s">
         <v>19</v>
       </c>
-      <c t="n" r="B11">
+      <c r="B11" t="n">
         <v>90.32258064516128</v>
       </c>
-      <c t="n" r="C11">
+      <c r="C11" t="n">
         <v>5.784648154399972</v>
       </c>
     </row>
-    <row spans="1:3" r="12">
-      <c t="s" r="A12" s="1">
+    <row r="12" spans="1:3">
+      <c s="1" r="A12" t="s">
         <v>29</v>
       </c>
-      <c t="n" r="B12">
+      <c r="B12" t="n">
         <v>86.89788053949904</v>
       </c>
-      <c t="n" r="C12">
+      <c r="C12" t="n">
         <v>3.6958964011015403</v>
       </c>
     </row>
-    <row spans="1:3" r="13">
-      <c t="s" r="A13" s="1">
+    <row r="13" spans="1:3">
+      <c s="1" r="A13" t="s">
         <v>9</v>
       </c>
-      <c t="n" r="B13">
+      <c r="B13" t="n">
         <v>84.21052631578947</v>
       </c>
-      <c t="n" r="C13">
+      <c r="C13" t="n">
         <v>2.5630013184811067</v>
       </c>
     </row>
-    <row spans="1:3" r="14">
-      <c t="s" r="A14" s="1">
+    <row r="14" spans="1:3">
+      <c s="1" r="A14" t="s">
         <v>27</v>
       </c>
-      <c t="n" r="B14">
+      <c r="B14" t="n">
         <v>90.78947368421053</v>
       </c>
-      <c t="n" r="C14">
+      <c r="C14" t="n">
         <v>0.17154465324478427</v>
       </c>
     </row>
-    <row spans="1:3" r="15">
-      <c t="s" r="A15" s="1">
+    <row r="15" spans="1:3">
+      <c s="1" r="A15" t="s">
         <v>7</v>
       </c>
-      <c t="n" r="B15">
+      <c r="B15" t="n">
         <v>80.5093555093555</v>
       </c>
-      <c t="n" r="C15">
+      <c r="C15" t="n">
         <v>1.390812017649007</v>
       </c>
     </row>
-    <row spans="1:3" r="16">
-      <c t="s" r="A16" s="1">
+    <row r="16" spans="1:3">
+      <c s="1" r="A16" t="s">
         <v>8</v>
       </c>
-      <c t="n" r="B16">
+      <c r="B16" t="n">
         <v>77.8987479586282</v>
       </c>
-      <c t="n" r="C16">
+      <c r="C16" t="n">
         <v>2.2081218050886764</v>
       </c>
     </row>
-    <row spans="1:3" r="17">
-      <c t="s" r="A17" s="1">
+    <row r="17" spans="1:3">
+      <c s="1" r="A17" t="s">
         <v>33</v>
       </c>
-      <c t="n" r="B17">
+      <c r="B17" t="n">
         <v>87.93774319066148</v>
       </c>
-      <c t="n" r="C17">
+      <c r="C17" t="n">
         <v>1.9321882952917213</v>
       </c>
     </row>
-    <row spans="1:3" r="18">
-      <c t="s" r="A18" s="1">
+    <row r="18" spans="1:3">
+      <c s="1" r="A18" t="s">
         <v>21</v>
       </c>
-      <c t="n" r="B18">
+      <c r="B18" t="n">
         <v>71.26168224299066</v>
       </c>
-      <c t="n" r="C18">
+      <c r="C18" t="n">
         <v>3.505976794019282</v>
       </c>
     </row>
-    <row spans="1:3" r="19">
-      <c t="s" r="A19" s="1">
+    <row r="19" spans="1:3">
+      <c s="1" r="A19" t="s">
         <v>11</v>
       </c>
-      <c t="n" r="B19">
+      <c r="B19" t="n">
         <v>78.28326180257511</v>
       </c>
-      <c t="n" r="C19">
+      <c r="C19" t="n">
         <v>2.4453800169787825</v>
       </c>
     </row>
-    <row spans="1:3" r="20">
-      <c t="s" r="A20" s="1">
+    <row r="20" spans="1:3">
+      <c s="1" r="A20" t="s">
         <v>45</v>
       </c>
-      <c t="n" r="B20">
+      <c r="B20" t="n">
         <v>78.57142857142857</v>
       </c>
-      <c t="n" r="C20">
+      <c r="C20" t="n">
         <v>3.632121693098543</v>
       </c>
     </row>
-    <row spans="1:3" r="21">
-      <c t="s" r="A21" s="1">
+    <row r="21" spans="1:3">
+      <c s="1" r="A21" t="s">
         <v>10</v>
       </c>
-      <c t="n" r="B21">
+      <c r="B21" t="n">
         <v>76.60702451954937</v>
       </c>
-      <c t="n" r="C21">
+      <c r="C21" t="n">
         <v>3.343405106866945</v>
       </c>
     </row>
-    <row spans="1:3" r="22">
-      <c t="s" r="A22" s="1">
+    <row r="22" spans="1:3">
+      <c s="1" r="A22" t="s">
         <v>39</v>
       </c>
-      <c t="n" r="B22">
+      <c r="B22" t="n">
         <v>84.09872547036213</v>
       </c>
-      <c t="n" r="C22">
+      <c r="C22" t="n">
         <v>3.9401900894274213</v>
       </c>
     </row>
-    <row spans="1:3" r="23">
-      <c t="s" r="A23" s="1">
+    <row r="23" spans="1:3">
+      <c s="1" r="A23" t="s">
         <v>43</v>
       </c>
-      <c t="n" r="B23">
+      <c r="B23" t="n">
         <v>84.1741901221455</v>
       </c>
-      <c t="n" r="C23">
+      <c r="C23" t="n">
         <v>1.013170610842692</v>
       </c>
     </row>
-    <row spans="1:3" r="24">
-      <c t="s" r="A24" s="1">
+    <row r="24" spans="1:3">
+      <c s="1" r="A24" t="s">
         <v>44</v>
       </c>
-      <c t="n" r="B24">
+      <c r="B24" t="n">
         <v>79.0224032586558</v>
       </c>
-      <c t="n" r="C24">
+      <c r="C24" t="n">
         <v>0.7908625589496129</v>
       </c>
     </row>
-    <row spans="1:3" r="25">
-      <c t="s" r="A25" s="1">
+    <row r="25" spans="1:3">
+      <c s="1" r="A25" t="s">
         <v>42</v>
       </c>
-      <c t="n" r="B25">
+      <c r="B25" t="n">
         <v>83.55932203389831</v>
       </c>
-      <c t="n" r="C25">
+      <c r="C25" t="n">
         <v>1.765565513212798</v>
       </c>
     </row>
-    <row spans="1:3" r="26">
-      <c t="s" r="A26" s="1">
+    <row r="26" spans="1:3">
+      <c s="1" r="A26" t="s">
         <v>20</v>
       </c>
-      <c t="n" r="B26">
+      <c r="B26" t="n">
         <v>86.40076886112446</v>
       </c>
-      <c t="n" r="C26">
+      <c r="C26" t="n">
         <v>2.639448533182737</v>
       </c>
     </row>
-    <row spans="1:3" r="27">
-      <c t="s" r="A27" s="1">
+    <row r="27" spans="1:3">
+      <c s="1" r="A27" t="s">
         <v>22</v>
       </c>
-      <c t="n" r="B27">
+      <c r="B27" t="n">
         <v>83.54898336414048</v>
       </c>
-      <c t="n" r="C27">
+      <c r="C27" t="n">
         <v>2.325921036487122</v>
       </c>
     </row>
-    <row spans="1:3" r="28">
-      <c t="s" r="A28" s="1">
+    <row r="28" spans="1:3">
+      <c s="1" r="A28" t="s">
         <v>5</v>
       </c>
-      <c t="n" r="B28">
+      <c r="B28" t="n">
         <v>82.27544910179641</v>
       </c>
-      <c t="n" r="C28">
+      <c r="C28" t="n">
         <v>2.386588526169974</v>
       </c>
     </row>
-    <row spans="1:3" r="29">
-      <c t="s" r="A29" s="1">
+    <row r="29" spans="1:3">
+      <c s="1" r="A29" t="s">
         <v>13</v>
       </c>
-      <c t="n" r="B29">
+      <c r="B29" t="n">
         <v>82.94930875576037</v>
       </c>
-      <c t="n" r="C29">
+      <c r="C29" t="n">
         <v>3.878773774155973</v>
       </c>
     </row>
-    <row spans="1:3" r="30">
-      <c t="s" r="A30" s="1">
+    <row r="30" spans="1:3">
+      <c s="1" r="A30" t="s">
         <v>4</v>
       </c>
-      <c t="n" r="B30">
+      <c r="B30" t="n">
         <v>85.0253807106599</v>
       </c>
-      <c t="n" r="C30">
+      <c r="C30" t="n">
         <v>1.9964901702806466</v>
       </c>
     </row>
-    <row spans="1:3" r="31">
-      <c t="s" r="A31" s="1">
+    <row r="31" spans="1:3">
+      <c s="1" r="A31" t="s">
         <v>24</v>
       </c>
-      <c t="n" r="B31">
+      <c r="B31" t="n">
         <v>89.0909090909091</v>
       </c>
-      <c t="n" r="C31">
+      <c r="C31" t="n">
         <v>2.4091040412349662</v>
       </c>
     </row>
-    <row spans="1:3" r="32">
-      <c t="s" r="A32" s="1">
+    <row r="32" spans="1:3">
+      <c s="1" r="A32" t="s">
         <v>41</v>
       </c>
-      <c t="n" r="B32">
+      <c r="B32" t="n">
         <v>88.42975206611571</v>
       </c>
-      <c t="n" r="C32">
+      <c r="C32" t="n">
         <v>0.5518696792864546</v>
       </c>
     </row>
-    <row spans="1:3" r="33">
-      <c t="s" r="A33" s="1">
+    <row r="33" spans="1:3">
+      <c s="1" r="A33" t="s">
         <v>25</v>
       </c>
-      <c t="n" r="B33">
+      <c r="B33" t="n">
         <v>87.6953125</v>
       </c>
-      <c t="n" r="C33">
+      <c r="C33" t="n">
         <v>4.835024065864382</v>
       </c>
     </row>
-    <row spans="1:3" r="34">
-      <c t="s" r="A34" s="1">
+    <row r="34" spans="1:3">
+      <c s="1" r="A34" t="s">
         <v>23</v>
       </c>
-      <c t="n" r="B34">
+      <c r="B34" t="n">
         <v>72.24416299726118</v>
       </c>
-      <c t="n" r="C34">
+      <c r="C34" t="n">
         <v>1.9638455018494472</v>
       </c>
     </row>
-    <row spans="1:3" r="35">
-      <c t="s" r="A35" s="1">
+    <row r="35" spans="1:3">
+      <c s="1" r="A35" t="s">
         <v>16</v>
       </c>
-      <c t="n" r="B35">
+      <c r="B35" t="n">
         <v>83.86292834890966</v>
       </c>
-      <c t="n" r="C35">
+      <c r="C35" t="n">
         <v>1.3852042225215384</v>
       </c>
     </row>
-    <row spans="1:3" r="36">
-      <c t="s" r="A36" s="1">
+    <row r="36" spans="1:3">
+      <c s="1" r="A36" t="s">
         <v>37</v>
       </c>
-      <c t="n" r="B36">
+      <c r="B36" t="n">
         <v>91.3913913913914</v>
       </c>
-      <c t="n" r="C36">
+      <c r="C36" t="n">
         <v>2.0128202560569033</v>
       </c>
     </row>
-    <row spans="1:3" r="37">
-      <c t="s" r="A37" s="1">
+    <row r="37" spans="1:3">
+      <c s="1" r="A37" t="s">
         <v>1</v>
       </c>
-      <c t="n" r="B37">
+      <c r="B37" t="n">
         <v>67.19554030874787</v>
       </c>
-      <c t="n" r="C37">
+      <c r="C37" t="n">
         <v>3.2080727098906614</v>
       </c>
     </row>
-    <row spans="1:3" r="38">
-      <c t="s" r="A38" s="1">
+    <row r="38" spans="1:3">
+      <c s="1" r="A38" t="s">
         <v>35</v>
       </c>
-      <c t="n" r="B38">
+      <c r="B38" t="n">
         <v>91.52542372881356</v>
       </c>
-      <c t="n" r="C38">
+      <c r="C38" t="n">
         <v>0.6412166202322017</v>
       </c>
     </row>
-    <row spans="1:3" r="39">
-      <c t="s" r="A39" s="1">
+    <row r="39" spans="1:3">
+      <c s="1" r="A39" t="s">
         <v>40</v>
       </c>
-      <c t="n" r="B39">
+      <c r="B39" t="n">
         <v>96.0</v>
       </c>
-      <c t="n" r="C39">
+      <c r="C39" t="n">
         <v>0.44300599380567335</v>
       </c>
     </row>
-    <row spans="1:3" r="40">
-      <c t="s" r="A40" s="1">
+    <row r="40" spans="1:3">
+      <c s="1" r="A40" t="s">
         <v>0</v>
       </c>
-      <c t="n" r="B40">
+      <c r="B40" t="n">
         <v>69.30860033726813</v>
       </c>
-      <c t="n" r="C40">
+      <c r="C40" t="n">
         <v>2.00161137722312</v>
       </c>
     </row>
-    <row spans="1:3" r="41">
-      <c t="s" r="A41" s="1">
+    <row r="41" spans="1:3">
+      <c s="1" r="A41" t="s">
         <v>14</v>
       </c>
-      <c t="n" r="B41">
+      <c r="B41" t="n">
         <v>86.09271523178808</v>
       </c>
-      <c t="n" r="C41">
+      <c r="C41" t="n">
         <v>0.47091351139931814</v>
       </c>
     </row>
-    <row spans="1:3" r="42">
-      <c t="s" r="A42" s="1">
+    <row r="42" spans="1:3">
+      <c s="1" r="A42" t="s">
         <v>17</v>
       </c>
-      <c t="n" r="B42">
+      <c r="B42" t="n">
         <v>91.06044154904089</v>
       </c>
-      <c t="n" r="C42">
+      <c r="C42" t="n">
         <v>1.1118360811806163</v>
       </c>
     </row>
-    <row spans="1:3" r="43">
-      <c t="s" r="A43" s="1">
+    <row r="43" spans="1:3">
+      <c s="1" r="A43" t="s">
         <v>2</v>
       </c>
-      <c t="n" r="B43">
+      <c r="B43" t="n">
         <v>88.5</v>
       </c>
-      <c t="n" r="C43">
+      <c r="C43" t="n">
         <v>4.2703721265535854</v>
       </c>
     </row>
-    <row spans="1:3" r="44">
-      <c t="s" r="A44" s="1">
+    <row r="44" spans="1:3">
+      <c s="1" r="A44" t="s">
         <v>18</v>
       </c>
-      <c t="n" r="B44">
+      <c r="B44" t="n">
         <v>89.79591836734694</v>
       </c>
-      <c t="n" r="C44">
+      <c r="C44" t="n">
         <v>0.06691970792759636</v>
       </c>
     </row>
-    <row spans="1:3" r="45">
-      <c t="s" r="A45" s="1">
+    <row r="45" spans="1:3">
+      <c s="1" r="A45" t="s">
         <v>38</v>
       </c>
-      <c t="n" r="B45">
+      <c r="B45" t="n">
         <v>67.59868421052632</v>
       </c>
-      <c t="n" r="C45">
+      <c r="C45" t="n">
         <v>1.1075916963162749</v>
       </c>
     </row>
-    <row spans="1:3" r="46">
-      <c t="s" r="A46" s="1">
+    <row r="46" spans="1:3">
+      <c s="1" r="A46" t="s">
         <v>32</v>
       </c>
-      <c t="n" r="B46">
+      <c r="B46" t="n">
         <v>79.54545454545455</v>
       </c>
-      <c t="n" r="C46">
+      <c r="C46" t="n">
         <v>4.909369380736884</v>
       </c>
     </row>
-    <row spans="1:3" r="47">
-      <c t="s" r="A47" s="1">
+    <row r="47" spans="1:3">
+      <c s="1" r="A47" t="s">
         <v>3</v>
       </c>
-      <c t="n" r="B47">
+      <c r="B47" t="n">
         <v>70.01455604075691</v>
       </c>
-      <c t="n" r="C47">
+      <c r="C47" t="n">
         <v>0.9431454354697535</v>
       </c>
     </row>

</xml_diff>